<commit_message>
fix: fix inheritance with dataclass with super post init
</commit_message>
<xml_diff>
--- a/docs/design_patterns.xlsx
+++ b/docs/design_patterns.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reighns/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reighns/gaohn/peekingduck-trainer/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73AD845A-9C6B-3546-A09E-CA26180794D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC5CC76-53BF-6443-B815-8E2BB62A4023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37980" yWindow="4340" windowWidth="27800" windowHeight="17500" activeTab="1" xr2:uid="{1260A8E3-4DB6-2148-8766-A729194B72FC}"/>
+    <workbookView xWindow="28800" yWindow="-1600" windowWidth="38400" windowHeight="21100" xr2:uid="{1260A8E3-4DB6-2148-8766-A729194B72FC}"/>
   </bookViews>
   <sheets>
     <sheet name="AISG" sheetId="1" r:id="rId1"/>
@@ -34,20 +34,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>http://karpathy.github.io/2019/04/25/recipe/</t>
   </si>
   <si>
-    <t>https://mail.google.com/mail/u/0/?ogbl&amp;zx=nuzc8hpm50l#inbox</t>
-  </si>
-  <si>
     <t>https://wordpress.deeplearning.ai/wp-content/uploads/2022/10/eBook-How-to-Build-a-Career-in-AI.pdf</t>
   </si>
   <si>
-    <t>https://github.com/gao-hongnan/peekingduck-trainer/tree/20221215-design-pattern</t>
-  </si>
-  <si>
     <t>https://github.com/aisingapore/PeekingDuck-Familiarization-YOLOv6/blob/main/Instructions.md</t>
   </si>
   <si>
@@ -69,12 +63,6 @@
     <t>https://github.com/gao-hongnan/peekingduck-trainer/blob/255cda60aacf51e9c2cd7f36929330b6441bd338/src/dataset.py</t>
   </si>
   <si>
-    <t>https://github.com/gao-hongnan/siim-isic-melanoma-classification/blob/master/src/make_folds.py</t>
-  </si>
-  <si>
-    <t>https://github.com/gao-hongnan/siim-isic-melanoma-classification/blob/master/src/prepare.py</t>
-  </si>
-  <si>
     <t>https://github.com/Lightning-AI/lightning/blob/master/examples/pl_loops/kfold.py</t>
   </si>
   <si>
@@ -196,6 +184,36 @@
   </si>
   <si>
     <t>Pros/Cons of Dependency Injection</t>
+  </si>
+  <si>
+    <t>https://torchmetrics.readthedocs.io/en/stable/classification/calibration_error.html</t>
+  </si>
+  <si>
+    <t>https://torchmetrics.readthedocs.io/en/stable/pages/overview.html#metriccollection</t>
+  </si>
+  <si>
+    <t>https://github.com/Lightning-AI/metrics/blob/master/src/torchmetrics/collections.py</t>
+  </si>
+  <si>
+    <t>https://github.com/Lightning-AI/metrics/blob/96862e0d8175da57f39e573230f6878892882062/src/torchmetrics/metric.py#L44</t>
+  </si>
+  <si>
+    <t>https://applyingml.com/resources/patterns/</t>
+  </si>
+  <si>
+    <t>https://www.educative.io/courses/machine-learning-system-design?aid=5082902844932096&amp;utm_source=google&amp;utm_medium=paid&amp;utm_campaign=machine-learning&amp;utm_term=machine%20learning%20system%20design&amp;utm_campaign=%5BTopics%5D+Machine+Learning&amp;utm_source=adwords&amp;utm_medium=ppc&amp;hsa_acc=5451446008&amp;hsa_cam=16394614703&amp;hsa_grp=136977609347&amp;hsa_ad=585425922123&amp;hsa_src=g&amp;hsa_tgt=kwd-302633670944&amp;hsa_kw=machine%20learning%20system%20design&amp;hsa_mt=b&amp;hsa_net=adwords&amp;hsa_ver=3&amp;gclid=Cj0KCQiA4OybBhCzARIsAIcfn9lahOmeXFWLhJ7fqpMJFfE9ciRpM9-lnwvKlgrHw2Z_QOTLi7oZR5gaAhoAEALw_wcB</t>
+  </si>
+  <si>
+    <t>https://medium.com/@upu1994/how-easy-is-making-custom-keras-callbacks-c771091602da</t>
+  </si>
+  <si>
+    <t>https://pytorch-lightning.readthedocs.io/en/stable/common/trainer.html</t>
+  </si>
+  <si>
+    <t>https://github.com/pytorch/vision/blob/main/references/classification/utils.py</t>
+  </si>
+  <si>
+    <t>https://github.com/Lightning-AI/lightning/blob/master/src/pytorch_lightning/callbacks/model_checkpoint.py</t>
   </si>
 </sst>
 </file>
@@ -562,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344C98D3-8419-C74B-8F9A-2A493B1F10F6}">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S33" sqref="S33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -622,22 +640,52 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -649,7 +697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D37910DF-0649-C143-9E74-87B9B046BE38}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -661,194 +709,194 @@
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>